<commit_message>
Adicionando script de monitoramento de jogos
</commit_message>
<xml_diff>
--- a/data/sent_games.xlsx
+++ b/data/sent_games.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>data</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo de Alerta</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>